<commit_message>
Alpha Descenso Recursivo: Faltan cosas
</commit_message>
<xml_diff>
--- a/informe-pl/compiler/src/descenso-recursivo/Gramática_Descenso_Recursivo.xlsx
+++ b/informe-pl/compiler/src/descenso-recursivo/Gramática_Descenso_Recursivo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NESTOR\Desktop\informe-pl-master\compiler\src\descenso-recursivo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NESTOR\Desktop\informe-pl\compiler\src\descenso-recursivo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A219DE8B-3183-4C62-AC88-5C256B04157E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE0FA01-8609-4487-93CB-B02FD3E7D050}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>input</t>
   </si>
@@ -102,6 +102,9 @@
     <t>INT_VAL, REAL_VAL, BOOL_VAL</t>
   </si>
   <si>
+    <t>ID, INT_VAL, REAL_VAL, BOOL_VAL, empty</t>
+  </si>
+  <si>
     <t>$</t>
   </si>
   <si>
@@ -184,36 +187,6 @@
   </si>
   <si>
     <t>d16</t>
-  </si>
-  <si>
-    <t>ID, INT_TYPE, REAL_TYPE, BOOL_TYPE</t>
-  </si>
-  <si>
-    <t>ID, INT_TYPE, REAL_TYPE, BOOL_TYPE, empty</t>
-  </si>
-  <si>
-    <t>INT_TYPE, REAL_TYPE, BOOL_TYPE</t>
-  </si>
-  <si>
-    <t>data_type</t>
-  </si>
-  <si>
-    <t>d21</t>
-  </si>
-  <si>
-    <t>d22</t>
-  </si>
-  <si>
-    <t>d23</t>
-  </si>
-  <si>
-    <t>INT_TYPE</t>
-  </si>
-  <si>
-    <t>REAL_TYPE</t>
-  </si>
-  <si>
-    <t>BOOL_TYPE</t>
   </si>
 </sst>
 </file>
@@ -409,6 +382,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -446,24 +434,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -846,7 +823,7 @@
   <dimension ref="A1:E106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,7 +841,7 @@
       <c r="B1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>21</v>
       </c>
     </row>
@@ -875,8 +852,8 @@
       <c r="B2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>24</v>
+      <c r="C2" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -886,10 +863,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>26</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -899,10 +876,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -914,8 +891,8 @@
       <c r="B5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>27</v>
+      <c r="C5" s="17" t="s">
+        <v>28</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -927,280 +904,255 @@
       <c r="B6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>28</v>
+      <c r="C6" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>29</v>
+      <c r="C7" s="18" t="s">
+        <v>30</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>2</v>
-      </c>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>31</v>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>52</v>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>25</v>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>54</v>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>2</v>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>1</v>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>12</v>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>9</v>
+      <c r="A18" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>11</v>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>27</v>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>2</v>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>23</v>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>7</v>
+      <c r="A24" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>15</v>
+      <c r="B27" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>28</v>
+      <c r="B28" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="B29" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>17</v>
+      <c r="B30" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>18</v>
-      </c>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="A33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>61</v>
-      </c>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>

</xml_diff>